<commit_message>
change name of file
</commit_message>
<xml_diff>
--- a/nba/players_for_fanduel.xlsx
+++ b/nba/players_for_fanduel.xlsx
@@ -7,14 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="PG" sheetId="1" r:id="rId1"/>
-    <sheet name="SG" sheetId="2" r:id="rId2"/>
-    <sheet name="PF" sheetId="3" r:id="rId3"/>
-    <sheet name="SF" sheetId="4" r:id="rId4"/>
-    <sheet name="C" sheetId="5" r:id="rId5"/>
-    <sheet name="All" sheetId="6" r:id="rId6"/>
-    <sheet name="STATS" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="ALL PLAYERS" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -5941,88 +5934,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>